<commit_message>
Addition of extra exchange reactions
</commit_message>
<xml_diff>
--- a/Data/Uptake_Secretion_Rates/specific_rates_ZeLa.xlsx
+++ b/Data/Uptake_Secretion_Rates/specific_rates_ZeLa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\DC\Manual curation_iCHO\Whole-Cell-Network-Reconstruction-for-CHO-cells_origin\Whole-Cell-Network-Reconstruction-for-CHO-cells\Data\Uptake_Secretion_Rates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablodigiusto/Documents/GitHub/Whole-Cell-Network-Reconstruction-for-CHO-cells/Data/Uptake_Secretion_Rates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A93456C-9A5D-478A-9A07-22DCE477DABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B394AD1A-830F-7A42-BFFA-529C5EC2C6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constraints" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="134">
   <si>
     <t>Batch ID</t>
   </si>
@@ -461,17 +461,26 @@
   </si>
   <si>
     <t>U8_P12_ZeLa</t>
+  </si>
+  <si>
+    <t>EX_5oxpro_e</t>
+  </si>
+  <si>
+    <t>EX_bhb_e</t>
+  </si>
+  <si>
+    <t>3-hydroxybutyric acid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -484,7 +493,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -499,7 +508,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -540,16 +549,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -558,7 +564,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -861,164 +867,168 @@
   <dimension ref="A1:AX36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="C1" s="6" t="s">
+    <row r="1" spans="1:50" ht="17">
+      <c r="A1" s="1"/>
+      <c r="C1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AH1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AM1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AN1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AO1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AP1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AR1" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AS1" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AT1" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AU1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AV1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="AW1" s="6" t="s">
+      <c r="AW1" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AX1" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>43</v>
+    <row r="2" spans="1:50" ht="17">
+      <c r="A2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
       </c>
       <c r="C2">
         <v>8.725471349882801E-4</v>
@@ -1165,8 +1175,8 @@
         <v>4.678699092829747E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:50" ht="17">
+      <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
@@ -1317,8 +1327,8 @@
         <v>1.6309321293234921E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:50" ht="17">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -1469,8 +1479,8 @@
         <v>6.1907096720173943E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:50" ht="17">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -1621,8 +1631,8 @@
         <v>5.8678357492971691E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:50" ht="17">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -1773,8 +1783,8 @@
         <v>-2.225194514252283E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:50" ht="17">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -1925,8 +1935,8 @@
         <v>-3.6745152432940881E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:50" ht="17">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -2077,8 +2087,8 @@
         <v>-1.239448664553687E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:50" ht="17">
+      <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B9" t="s">
@@ -2229,8 +2239,8 @@
         <v>3.1057891544798251E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:50" ht="17">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
@@ -2381,8 +2391,8 @@
         <v>-8.0483742697861737E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:50" ht="17">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
@@ -2533,11 +2543,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:50" ht="17">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C12">
@@ -2685,11 +2695,11 @@
         <v>-1.4294645649474479E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:50" ht="17">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C13">
@@ -2837,11 +2847,11 @@
         <v>-2.617404771870576E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:50" ht="17">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C14">
@@ -2989,11 +2999,11 @@
         <v>5.6307575261455782E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:50" ht="17">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C15">
@@ -3141,11 +3151,11 @@
         <v>-0.41908151314964998</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:50" ht="17">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C16">
@@ -3293,11 +3303,11 @@
         <v>2.9889345646524892E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:50" ht="17">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C17">
@@ -3445,11 +3455,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:50" ht="17">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C18">
@@ -3597,11 +3607,11 @@
         <v>1.367817293489986E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:50" ht="17">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C19">
@@ -3749,11 +3759,11 @@
         <v>-5.536957396764131E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:50" ht="17">
+      <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C20">
@@ -3901,11 +3911,11 @@
         <v>-2.748837048452996E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:50" ht="17">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C21">
@@ -4053,8 +4063,8 @@
         <v>-7.8446139202449274E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:50" ht="17">
+      <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C22">
@@ -4202,11 +4212,11 @@
         <v>1.082337612724754E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:50" ht="17">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C23">
@@ -4354,11 +4364,11 @@
         <v>6.9991409536328836E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:50" ht="17">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C24">
@@ -4506,11 +4516,11 @@
         <v>-1.236413057012976E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:50" ht="17">
+      <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C25">
@@ -4658,11 +4668,11 @@
         <v>7.5550846125897113E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:50" ht="17">
+      <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C26">
@@ -4810,8 +4820,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:50" ht="17">
+      <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B27" t="s">
@@ -4962,11 +4972,11 @@
         <v>-1.1499871889322239E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:50" ht="17">
+      <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C28">
@@ -5114,11 +5124,11 @@
         <v>-1.715732893481037E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:50" ht="17">
+      <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C29">
@@ -5266,9 +5276,12 @@
         <v>1.833388519323994E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:50" ht="17">
+      <c r="A30" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="C30">
         <v>2.5373245858114041E-2</v>
@@ -5415,8 +5428,8 @@
         <v>1.6433747760565241E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:50" ht="17">
+      <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
@@ -5567,8 +5580,8 @@
         <v>2.0246525205951998E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:50" ht="17">
+      <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
@@ -5719,8 +5732,8 @@
         <v>-6.2260297589143774E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:50" ht="17">
+      <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B33" t="s">
@@ -5871,8 +5884,8 @@
         <v>-3.0188761820048359E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:50" ht="17">
+      <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B34" t="s">
@@ -6023,8 +6036,8 @@
         <v>-4.0750884804539294E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:50" ht="17">
+      <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B35" t="s">
@@ -6175,8 +6188,8 @@
         <v>-1.061881856703392E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:50" ht="17">
+      <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B36" t="s">
@@ -6338,29 +6351,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C50" sqref="C3:C50"/>
+    <sheetView zoomScale="108" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.25" customWidth="1"/>
-    <col min="12" max="21" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="25" max="29" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1640625" customWidth="1"/>
+    <col min="12" max="21" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="29" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38">
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
       <c r="E1" t="s">
         <v>49</v>
       </c>
@@ -6388,56 +6404,59 @@
       <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AC1" t="s">
         <v>68</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="2" t="s">
         <v>70</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="AG1" t="s">
         <v>71</v>
@@ -6458,14 +6477,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" ht="17">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
         <v>43</v>
       </c>
@@ -6572,14 +6591,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:38" ht="17">
+      <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="4" t="str">
+      <c r="C3" s="3" t="str">
         <f>_xlfn.CONCAT(A3,"_",B3,"_ZeLa")</f>
         <v>U1_P2_ZeLa</v>
       </c>
@@ -6689,14 +6708,14 @@
         <v>-2.394258016093268E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:38" ht="17">
+      <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="4" t="str">
+      <c r="C4" s="3" t="str">
         <f>_xlfn.CONCAT(A4,"_",B4,"_ZeLa")</f>
         <v>U1_P14_ZeLa</v>
       </c>
@@ -6806,14 +6825,14 @@
         <v>-5.7811087090048022E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:38" ht="17">
+      <c r="A5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="4" t="str">
+      <c r="C5" s="3" t="str">
         <f>_xlfn.CONCAT(A5,"_",B5,"_ZeLa")</f>
         <v>U1_P4_ZeLa</v>
       </c>
@@ -6923,14 +6942,14 @@
         <v>-8.7350090315142081E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:38" ht="17">
+      <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="4" t="str">
+      <c r="C6" s="3" t="str">
         <f t="shared" ref="C6:C50" si="0">_xlfn.CONCAT(A6,"_",B6,"_ZeLa")</f>
         <v>U1_P6_ZeLa</v>
       </c>
@@ -7040,14 +7059,14 @@
         <v>-2.739606206083029E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:38" ht="17">
+      <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="4" t="str">
+      <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U1_P8_ZeLa</v>
       </c>
@@ -7157,14 +7176,14 @@
         <v>-8.0603925299383653E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:38" ht="17">
+      <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="4" t="str">
+      <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U1_P12_ZeLa</v>
       </c>
@@ -7274,14 +7293,14 @@
         <v>-4.9724015813026163E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:38" ht="17">
+      <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="4" t="str">
+      <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U2_P2_ZeLa</v>
       </c>
@@ -7391,14 +7410,14 @@
         <v>-1.7992427431385411E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:38" ht="17">
+      <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="4" t="str">
+      <c r="C10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U2_P14_ZeLa</v>
       </c>
@@ -7508,14 +7527,14 @@
         <v>6.2513924198423477E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:38" ht="17">
+      <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="4" t="str">
+      <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U2_P4_ZeLa</v>
       </c>
@@ -7625,14 +7644,14 @@
         <v>-8.973357193721547E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:38" ht="17">
+      <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="4" t="str">
+      <c r="C12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U2_P6_ZeLa</v>
       </c>
@@ -7742,14 +7761,14 @@
         <v>-2.910666896648019E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:38" ht="17">
+      <c r="A13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="4" t="str">
+      <c r="C13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U2_P8_ZeLa</v>
       </c>
@@ -7859,14 +7878,14 @@
         <v>-4.4322977222303614E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:38" ht="17">
+      <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="4" t="str">
+      <c r="C14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U2_P12_ZeLa</v>
       </c>
@@ -7976,14 +7995,14 @@
         <v>-1.119590966044086E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:38" ht="17">
+      <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="4" t="str">
+      <c r="C15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U3_P2_ZeLa</v>
       </c>
@@ -8093,14 +8112,14 @@
         <v>-3.2740744965958401E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:38" ht="17">
+      <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="4" t="str">
+      <c r="C16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U3_P14_ZeLa</v>
       </c>
@@ -8210,14 +8229,14 @@
         <v>2.108647002827947E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:38" ht="17">
+      <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="4" t="str">
+      <c r="C17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U3_P4_ZeLa</v>
       </c>
@@ -8327,14 +8346,14 @@
         <v>-7.8000761323300562E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:38" ht="17">
+      <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="4" t="str">
+      <c r="C18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U3_P6_ZeLa</v>
       </c>
@@ -8444,14 +8463,14 @@
         <v>-4.3677123210435504E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:38" ht="17">
+      <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="4" t="str">
+      <c r="C19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U3_P8_ZeLa</v>
       </c>
@@ -8561,14 +8580,14 @@
         <v>-1.494487694035185E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:38" ht="17">
+      <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="4" t="str">
+      <c r="C20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U3_P12_ZeLa</v>
       </c>
@@ -8678,14 +8697,14 @@
         <v>-1.4700569816381E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:38" ht="17">
+      <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="4" t="str">
+      <c r="C21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U4_P2_ZeLa</v>
       </c>
@@ -8795,14 +8814,14 @@
         <v>-2.1407285121745031E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:38" ht="17">
+      <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="4" t="str">
+      <c r="C22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U4_P14_ZeLa</v>
       </c>
@@ -8912,14 +8931,14 @@
         <v>-4.287498729536946E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:38" ht="17">
+      <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="4" t="str">
+      <c r="C23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U4_P4_ZeLa</v>
       </c>
@@ -9029,14 +9048,14 @@
         <v>-5.9662036941974771E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:38" ht="17">
+      <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="4" t="str">
+      <c r="C24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U4_P6_ZeLa</v>
       </c>
@@ -9146,14 +9165,14 @@
         <v>-9.3799181830686931E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:38" ht="17">
+      <c r="A25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="4" t="str">
+      <c r="C25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U4_P8_ZeLa</v>
       </c>
@@ -9263,14 +9282,14 @@
         <v>1.6558240501996389E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:38" ht="17">
+      <c r="A26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="4" t="str">
+      <c r="C26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U4_P12_ZeLa</v>
       </c>
@@ -9380,14 +9399,14 @@
         <v>-4.1292067151742686E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:38" ht="17">
+      <c r="A27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="4" t="str">
+      <c r="C27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U5_P2_ZeLa</v>
       </c>
@@ -9497,14 +9516,14 @@
         <v>-4.0988087685284577E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+    <row r="28" spans="1:38" ht="17">
+      <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="4" t="str">
+      <c r="C28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U5_P14_ZeLa</v>
       </c>
@@ -9614,14 +9633,14 @@
         <v>-2.6594648574057448E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:38" ht="17">
+      <c r="A29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="4" t="str">
+      <c r="C29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U5_P4_ZeLa</v>
       </c>
@@ -9731,14 +9750,14 @@
         <v>-3.288631365252447E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+    <row r="30" spans="1:38" ht="17">
+      <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="4" t="str">
+      <c r="C30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U5_P6_ZeLa</v>
       </c>
@@ -9848,14 +9867,14 @@
         <v>-1.034044648615234E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:38" ht="17">
+      <c r="A31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="4" t="str">
+      <c r="C31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U5_P8_ZeLa</v>
       </c>
@@ -9965,14 +9984,14 @@
         <v>-1.2923002407489251E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+    <row r="32" spans="1:38" ht="17">
+      <c r="A32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="4" t="str">
+      <c r="C32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U5_P12_ZeLa</v>
       </c>
@@ -10082,14 +10101,14 @@
         <v>-8.2261635721410827E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+    <row r="33" spans="1:38" ht="17">
+      <c r="A33" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="4" t="str">
+      <c r="C33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U6_P2_ZeLa</v>
       </c>
@@ -10199,14 +10218,14 @@
         <v>-4.0473524949711064E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:38" ht="17">
+      <c r="A34" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="4" t="str">
+      <c r="C34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U6_P14_ZeLa</v>
       </c>
@@ -10316,14 +10335,14 @@
         <v>-6.4905776929123605E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+    <row r="35" spans="1:38" ht="17">
+      <c r="A35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="4" t="str">
+      <c r="C35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U6_P4_ZeLa</v>
       </c>
@@ -10433,14 +10452,14 @@
         <v>-6.4072310944925347E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+    <row r="36" spans="1:38" ht="17">
+      <c r="A36" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="4" t="str">
+      <c r="C36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U6_P6_ZeLa</v>
       </c>
@@ -10550,14 +10569,14 @@
         <v>-7.5857600622880614E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:38" ht="17">
+      <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="4" t="str">
+      <c r="C37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U6_P8_ZeLa</v>
       </c>
@@ -10667,14 +10686,14 @@
         <v>5.2669678349986102E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:38" ht="17">
+      <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="4" t="str">
+      <c r="C38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U6_P12_ZeLa</v>
       </c>
@@ -10784,14 +10803,14 @@
         <v>-3.0223006853061919E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="1:38" ht="17">
+      <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="4" t="str">
+      <c r="C39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U7_P2_ZeLa</v>
       </c>
@@ -10901,14 +10920,14 @@
         <v>-1.679793641233097E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:38" ht="17">
+      <c r="A40" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="4" t="str">
+      <c r="C40" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U7_P14_ZeLa</v>
       </c>
@@ -11018,14 +11037,14 @@
         <v>-6.5422586650154882E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:38" ht="17">
+      <c r="A41" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="4" t="str">
+      <c r="C41" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U7_P4_ZeLa</v>
       </c>
@@ -11135,14 +11154,14 @@
         <v>-6.5137206324637192E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:38" ht="17">
+      <c r="A42" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="4" t="str">
+      <c r="C42" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U7_P6_ZeLa</v>
       </c>
@@ -11252,14 +11271,14 @@
         <v>-9.1993649546934439E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:38" ht="17">
+      <c r="A43" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C43" s="4" t="str">
+      <c r="C43" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U7_P8_ZeLa</v>
       </c>
@@ -11369,14 +11388,14 @@
         <v>2.3806784040155552E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:38" ht="17">
+      <c r="A44" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="4" t="str">
+      <c r="C44" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U7_P12_ZeLa</v>
       </c>
@@ -11486,14 +11505,14 @@
         <v>-2.838376937928472E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+    <row r="45" spans="1:38" ht="17">
+      <c r="A45" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="4" t="str">
+      <c r="C45" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U8_P2_ZeLa</v>
       </c>
@@ -11603,14 +11622,14 @@
         <v>-1.9629538525589279E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+    <row r="46" spans="1:38" ht="17">
+      <c r="A46" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="4" t="str">
+      <c r="C46" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U8_P14_ZeLa</v>
       </c>
@@ -11720,14 +11739,14 @@
         <v>-2.1745328540107541E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:38" ht="17">
+      <c r="A47" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="4" t="str">
+      <c r="C47" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U8_P4_ZeLa</v>
       </c>
@@ -11837,14 +11856,14 @@
         <v>-5.278989319216696E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+    <row r="48" spans="1:38" ht="17">
+      <c r="A48" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="4" t="str">
+      <c r="C48" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U8_P6_ZeLa</v>
       </c>
@@ -11954,14 +11973,14 @@
         <v>-1.004986670066592E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:38" ht="17">
+      <c r="A49" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="4" t="str">
+      <c r="C49" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U8_P8_ZeLa</v>
       </c>
@@ -12071,14 +12090,14 @@
         <v>-1.0237085773417099E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+    <row r="50" spans="1:38" ht="17">
+      <c r="A50" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="4" t="str">
+      <c r="C50" s="3" t="str">
         <f t="shared" si="0"/>
         <v>U8_P12_ZeLa</v>
       </c>

</xml_diff>

<commit_message>
Minor updates on ZeLa datasets
</commit_message>
<xml_diff>
--- a/Data/Uptake_Secretion_Rates/specific_rates_ZeLa.xlsx
+++ b/Data/Uptake_Secretion_Rates/specific_rates_ZeLa.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablodigiusto/Documents/GitHub/Whole-Cell-Network-Reconstruction-for-CHO-cells/Data/Uptake_Secretion_Rates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\DC\Manual curation_iCHO\Whole-Cell-Network-Reconstruction-for-CHO-cells_origin\Whole-Cell-Network-Reconstruction-for-CHO-cells\Data\Uptake_Secretion_Rates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B394AD1A-830F-7A42-BFFA-529C5EC2C6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CA6A67-34CC-46B6-9227-FA64DCAFBEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constraints" sheetId="2" r:id="rId1"/>
     <sheet name="Specific Rates" sheetId="1" r:id="rId2"/>
+    <sheet name="Constraints_U1_U3" sheetId="3" r:id="rId3"/>
+    <sheet name="Constraints_U4_U8" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="142">
   <si>
     <t>Batch ID</t>
   </si>
@@ -470,17 +472,46 @@
   </si>
   <si>
     <t>3-hydroxybutyric acid</t>
+  </si>
+  <si>
+    <t>Reaction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Metabolite</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2 to P4</t>
+  </si>
+  <si>
+    <t>P4 to P6</t>
+  </si>
+  <si>
+    <t>P6 to P8</t>
+  </si>
+  <si>
+    <t>P2 to P4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Measured growth rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>biomass</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -493,7 +524,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -508,7 +539,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -522,7 +553,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -545,11 +576,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -562,9 +604,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -866,18 +911,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F361205-3DFF-4D40-8261-D833A0E98908}">
   <dimension ref="A1:AX36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:AX4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="17">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
       <c r="C1" s="5" t="s">
         <v>83</v>
       </c>
@@ -1023,7 +1073,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:50" ht="17">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>133</v>
       </c>
@@ -1175,7 +1225,7 @@
         <v>4.678699092829747E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="17">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
@@ -1327,7 +1377,7 @@
         <v>1.6309321293234921E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="17">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1479,7 +1529,7 @@
         <v>6.1907096720173943E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:50" ht="17">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1631,7 +1681,7 @@
         <v>5.8678357492971691E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="17">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1783,7 +1833,7 @@
         <v>-2.225194514252283E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:50" ht="17">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1935,7 +1985,7 @@
         <v>-3.6745152432940881E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:50" ht="17">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2087,7 +2137,7 @@
         <v>-1.239448664553687E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:50" ht="17">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -2239,7 +2289,7 @@
         <v>3.1057891544798251E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:50" ht="17">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2391,7 +2441,7 @@
         <v>-8.0483742697861737E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:50" ht="17">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2543,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:50" ht="17">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2695,7 +2745,7 @@
         <v>-1.4294645649474479E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:50" ht="17">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2847,7 +2897,7 @@
         <v>-2.617404771870576E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:50" ht="17">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2999,7 +3049,7 @@
         <v>5.6307575261455782E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:50" ht="17">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3151,7 +3201,7 @@
         <v>-0.41908151314964998</v>
       </c>
     </row>
-    <row r="16" spans="1:50" ht="17">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -3303,7 +3353,7 @@
         <v>2.9889345646524892E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:50" ht="17">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3455,7 +3505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:50" ht="17">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -3607,7 +3657,7 @@
         <v>1.367817293489986E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:50" ht="17">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -3759,7 +3809,7 @@
         <v>-5.536957396764131E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:50" ht="17">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -3911,7 +3961,7 @@
         <v>-2.748837048452996E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:50" ht="17">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -4063,7 +4113,7 @@
         <v>-7.8446139202449274E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:50" ht="17">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -4212,7 +4262,7 @@
         <v>1.082337612724754E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:50" ht="17">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -4364,7 +4414,7 @@
         <v>6.9991409536328836E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:50" ht="17">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -4516,7 +4566,7 @@
         <v>-1.236413057012976E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:50" ht="17">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -4668,7 +4718,7 @@
         <v>7.5550846125897113E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:50" ht="17">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -4820,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:50" ht="17">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -4972,7 +5022,7 @@
         <v>-1.1499871889322239E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:50" ht="17">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -5124,7 +5174,7 @@
         <v>-1.715732893481037E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:50" ht="17">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -5276,7 +5326,7 @@
         <v>1.833388519323994E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:50" ht="17">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -5428,7 +5478,7 @@
         <v>1.6433747760565241E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:50" ht="17">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -5580,7 +5630,7 @@
         <v>2.0246525205951998E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:50" ht="17">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -5732,7 +5782,7 @@
         <v>-6.2260297589143774E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:50" ht="17">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -5884,7 +5934,7 @@
         <v>-3.0188761820048359E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:50" ht="17">
+    <row r="34" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -6036,7 +6086,7 @@
         <v>-4.0750884804539294E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:50" ht="17">
+    <row r="35" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -6188,7 +6238,7 @@
         <v>-1.061881856703392E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:50" ht="17">
+    <row r="36" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -6355,25 +6405,25 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.1640625" customWidth="1"/>
-    <col min="12" max="21" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="29" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.125" customWidth="1"/>
+    <col min="12" max="21" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="29" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>132</v>
       </c>
@@ -6477,7 +6527,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="17">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -6591,7 +6641,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="17">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
@@ -6708,7 +6758,7 @@
         <v>-2.394258016093268E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="17">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -6825,7 +6875,7 @@
         <v>-5.7811087090048022E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="17">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>34</v>
       </c>
@@ -6942,7 +6992,7 @@
         <v>-8.7350090315142081E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="17">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
@@ -7059,7 +7109,7 @@
         <v>-2.739606206083029E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="17">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
@@ -7176,7 +7226,7 @@
         <v>-8.0603925299383653E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="17">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
@@ -7293,7 +7343,7 @@
         <v>-4.9724015813026163E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="17">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
@@ -7410,7 +7460,7 @@
         <v>-1.7992427431385411E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="17">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
@@ -7527,7 +7577,7 @@
         <v>6.2513924198423477E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="17">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
@@ -7644,7 +7694,7 @@
         <v>-8.973357193721547E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="17">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -7761,7 +7811,7 @@
         <v>-2.910666896648019E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="17">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>35</v>
       </c>
@@ -7878,7 +7928,7 @@
         <v>-4.4322977222303614E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="17">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
@@ -7995,7 +8045,7 @@
         <v>-1.119590966044086E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="17">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
@@ -8112,7 +8162,7 @@
         <v>-3.2740744965958401E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="17">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
@@ -8229,7 +8279,7 @@
         <v>2.108647002827947E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="17">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
@@ -8346,7 +8396,7 @@
         <v>-7.8000761323300562E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="17">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
@@ -8463,7 +8513,7 @@
         <v>-4.3677123210435504E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="17">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
@@ -8580,7 +8630,7 @@
         <v>-1.494487694035185E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="17">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
@@ -8697,7 +8747,7 @@
         <v>-1.4700569816381E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="17">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
@@ -8814,7 +8864,7 @@
         <v>-2.1407285121745031E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="17">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
@@ -8931,7 +8981,7 @@
         <v>-4.287498729536946E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="17">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
@@ -9048,7 +9098,7 @@
         <v>-5.9662036941974771E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="17">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
@@ -9165,7 +9215,7 @@
         <v>-9.3799181830686931E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="17">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>37</v>
       </c>
@@ -9282,7 +9332,7 @@
         <v>1.6558240501996389E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="17">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>37</v>
       </c>
@@ -9399,7 +9449,7 @@
         <v>-4.1292067151742686E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:38" ht="17">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>38</v>
       </c>
@@ -9516,7 +9566,7 @@
         <v>-4.0988087685284577E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:38" ht="17">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
@@ -9633,7 +9683,7 @@
         <v>-2.6594648574057448E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="17">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>38</v>
       </c>
@@ -9750,7 +9800,7 @@
         <v>-3.288631365252447E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:38" ht="17">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
@@ -9867,7 +9917,7 @@
         <v>-1.034044648615234E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:38" ht="17">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>38</v>
       </c>
@@ -9984,7 +10034,7 @@
         <v>-1.2923002407489251E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:38" ht="17">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>38</v>
       </c>
@@ -10101,7 +10151,7 @@
         <v>-8.2261635721410827E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:38" ht="17">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>39</v>
       </c>
@@ -10218,7 +10268,7 @@
         <v>-4.0473524949711064E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:38" ht="17">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>39</v>
       </c>
@@ -10335,7 +10385,7 @@
         <v>-6.4905776929123605E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:38" ht="17">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>39</v>
       </c>
@@ -10452,7 +10502,7 @@
         <v>-6.4072310944925347E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:38" ht="17">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>39</v>
       </c>
@@ -10569,7 +10619,7 @@
         <v>-7.5857600622880614E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:38" ht="17">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
@@ -10686,7 +10736,7 @@
         <v>5.2669678349986102E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:38" ht="17">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
@@ -10803,7 +10853,7 @@
         <v>-3.0223006853061919E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:38" ht="17">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
@@ -10920,7 +10970,7 @@
         <v>-1.679793641233097E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:38" ht="17">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>40</v>
       </c>
@@ -11037,7 +11087,7 @@
         <v>-6.5422586650154882E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:38" ht="17">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>40</v>
       </c>
@@ -11154,7 +11204,7 @@
         <v>-6.5137206324637192E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:38" ht="17">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>40</v>
       </c>
@@ -11271,7 +11321,7 @@
         <v>-9.1993649546934439E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:38" ht="17">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>40</v>
       </c>
@@ -11388,7 +11438,7 @@
         <v>2.3806784040155552E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:38" ht="17">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>40</v>
       </c>
@@ -11505,7 +11555,7 @@
         <v>-2.838376937928472E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:38" ht="17">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>41</v>
       </c>
@@ -11622,7 +11672,7 @@
         <v>-1.9629538525589279E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:38" ht="17">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>41</v>
       </c>
@@ -11739,7 +11789,7 @@
         <v>-2.1745328540107541E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:38" ht="17">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>41</v>
       </c>
@@ -11856,7 +11906,7 @@
         <v>-5.278989319216696E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:38" ht="17">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>41</v>
       </c>
@@ -11973,7 +12023,7 @@
         <v>-1.004986670066592E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:38" ht="17">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>41</v>
       </c>
@@ -12090,7 +12140,7 @@
         <v>-1.0237085773417099E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:38" ht="17">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>41</v>
       </c>
@@ -12212,4 +12262,1298 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63928BBD-E54E-4F85-9CDC-9951C0272260}">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2">
+        <v>1.5922128800968721E-3</v>
+      </c>
+      <c r="D2">
+        <v>2.6786978428644742E-4</v>
+      </c>
+      <c r="E2">
+        <v>5.6813518985585716E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3">
+        <v>4.4243872452972892E-2</v>
+      </c>
+      <c r="D3">
+        <v>-2.5434889710600561E-3</v>
+      </c>
+      <c r="E3">
+        <v>3.3191077275790112E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>5.5371516817346396E-4</v>
+      </c>
+      <c r="D4">
+        <v>4.2769114700457224E-3</v>
+      </c>
+      <c r="E4">
+        <v>0.1113272138979865</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>2.2113180557447619E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.5777635355535978E-3</v>
+      </c>
+      <c r="E5">
+        <v>-3.5761326495362712E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>-7.1609720609032189E-3</v>
+      </c>
+      <c r="D6">
+        <v>-2.5076473455946332E-3</v>
+      </c>
+      <c r="E6">
+        <v>-4.8064700580554868E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7">
+        <v>-4.2913482556427893E-2</v>
+      </c>
+      <c r="D7">
+        <v>-1.0211891024983381E-2</v>
+      </c>
+      <c r="E7">
+        <v>-1.8822774807503349E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8">
+        <v>7.5104269563984723E-3</v>
+      </c>
+      <c r="D8">
+        <v>-1.037808738993666E-3</v>
+      </c>
+      <c r="E8">
+        <v>-1.1266388859545491E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>5.9288916126592659E-4</v>
+      </c>
+      <c r="D9">
+        <v>7.5752910264909035E-4</v>
+      </c>
+      <c r="E9">
+        <v>5.2900384840701628E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>2.8626154445188729E-3</v>
+      </c>
+      <c r="D10">
+        <v>1.636962930264567E-3</v>
+      </c>
+      <c r="E10">
+        <v>7.7913220554655504E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <v>-1.4796534266201589E-3</v>
+      </c>
+      <c r="D11">
+        <v>-2.246573263411703E-4</v>
+      </c>
+      <c r="E11">
+        <v>-6.7613548460312924E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>2.0017059268571401E-2</v>
+      </c>
+      <c r="D12">
+        <v>4.5273490106371968E-3</v>
+      </c>
+      <c r="E12">
+        <v>-3.9886328492939632E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13">
+        <v>1.237207650985519E-2</v>
+      </c>
+      <c r="D13">
+        <v>5.776483618620442E-3</v>
+      </c>
+      <c r="E13">
+        <v>4.289498300913794E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14">
+        <v>8.1491363279339061E-5</v>
+      </c>
+      <c r="D14">
+        <v>-1.4776782981603119E-5</v>
+      </c>
+      <c r="E14">
+        <v>6.7398204555731177E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15">
+        <v>-0.22776992406971991</v>
+      </c>
+      <c r="D15">
+        <v>-8.3688783363159894E-2</v>
+      </c>
+      <c r="E15">
+        <v>-0.51498110200420044</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16">
+        <v>5.4832905915170481E-3</v>
+      </c>
+      <c r="D16">
+        <v>8.1384301925264567E-4</v>
+      </c>
+      <c r="E16">
+        <v>3.5277733949710569E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17">
+        <v>-4.5813349498808463E-2</v>
+      </c>
+      <c r="D17">
+        <v>-3.2692500121940561E-3</v>
+      </c>
+      <c r="E17">
+        <v>2.9118613223681251E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18">
+        <v>5.6977051556665109E-3</v>
+      </c>
+      <c r="D18">
+        <v>3.507351449171245E-3</v>
+      </c>
+      <c r="E18">
+        <v>4.6700905597627769E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>-2.6867653228781672E-3</v>
+      </c>
+      <c r="D19">
+        <v>-1.0830523960134049E-3</v>
+      </c>
+      <c r="E19">
+        <v>-1.8741886452543911E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20">
+        <v>-1.0682217596883509E-3</v>
+      </c>
+      <c r="D20">
+        <v>-3.8994824304673068E-4</v>
+      </c>
+      <c r="E20">
+        <v>5.1415492306777885E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21">
+        <v>-6.1837475424657484E-3</v>
+      </c>
+      <c r="D21">
+        <v>-2.8846147264317279E-3</v>
+      </c>
+      <c r="E21">
+        <v>-8.6461810289344531E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>2.5412321366991849E-4</v>
+      </c>
+      <c r="D22">
+        <v>6.2715661976157585E-4</v>
+      </c>
+      <c r="E22">
+        <v>8.8625137098353995E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23">
+        <v>0.32387002276580051</v>
+      </c>
+      <c r="D23">
+        <v>4.8595818984263427E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.13397716328206019</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24">
+        <v>-1.025101917436293E-2</v>
+      </c>
+      <c r="D24">
+        <v>-4.5083044944140838E-3</v>
+      </c>
+      <c r="E24">
+        <v>-1.551534841006442E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25">
+        <v>-1.0218111051851121E-2</v>
+      </c>
+      <c r="D25">
+        <v>-3.2936591632474511E-3</v>
+      </c>
+      <c r="E25">
+        <v>-7.7146095294143742E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27">
+        <v>-3.320941347783218E-3</v>
+      </c>
+      <c r="D27">
+        <v>-1.127251054357995E-3</v>
+      </c>
+      <c r="E27">
+        <v>-3.0168683218575209E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28">
+        <v>-4.0298053601933864E-3</v>
+      </c>
+      <c r="D28">
+        <v>-1.7370005507132951E-3</v>
+      </c>
+      <c r="E28">
+        <v>-4.2020511436277773E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29">
+        <v>-1.555455355323849E-2</v>
+      </c>
+      <c r="D29">
+        <v>-3.4187081995964898E-3</v>
+      </c>
+      <c r="E29">
+        <v>-6.2783697252822178E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30">
+        <v>4.5043775912787373E-3</v>
+      </c>
+      <c r="D30">
+        <v>8.04594995683818E-4</v>
+      </c>
+      <c r="E30">
+        <v>5.0742858220845987E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31">
+        <v>1.605664434930423E-3</v>
+      </c>
+      <c r="D31">
+        <v>-3.1651322992622549E-3</v>
+      </c>
+      <c r="E31">
+        <v>-3.0020692069349479E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32">
+        <v>-2.555457531768545E-2</v>
+      </c>
+      <c r="D32">
+        <v>-1.1007110111017401E-2</v>
+      </c>
+      <c r="E32">
+        <v>-2.0412059886923621E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33">
+        <v>-7.7902674403486508E-3</v>
+      </c>
+      <c r="D33">
+        <v>-2.5646742614420532E-3</v>
+      </c>
+      <c r="E33">
+        <v>-4.1154348314979333E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34">
+        <v>-1.4836707615867909E-3</v>
+      </c>
+      <c r="D34">
+        <v>-8.9773432150042803E-4</v>
+      </c>
+      <c r="E34">
+        <v>-3.9075557071319876E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35">
+        <v>-4.6827736256816127E-3</v>
+      </c>
+      <c r="D35">
+        <v>-1.037340166232079E-3</v>
+      </c>
+      <c r="E35">
+        <v>-3.630985942990001E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36">
+        <v>-8.5028141191886026E-3</v>
+      </c>
+      <c r="D36">
+        <v>-3.3393284745915331E-3</v>
+      </c>
+      <c r="E36">
+        <v>-9.1458557308401935E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37">
+        <v>0.1581623286936639</v>
+      </c>
+      <c r="D37">
+        <v>5.2167312256431821E-2</v>
+      </c>
+      <c r="E37">
+        <v>-5.5481926702465018E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622D85ED-938F-4403-A818-A71CD1E347C1}">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2">
+        <v>-7.5150308400904437E-6</v>
+      </c>
+      <c r="D2">
+        <v>1.9433653477551801E-4</v>
+      </c>
+      <c r="E2">
+        <v>-8.2031918543681493E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3">
+        <v>3.9768081088773798E-2</v>
+      </c>
+      <c r="D3">
+        <v>-4.2047796576285101E-2</v>
+      </c>
+      <c r="E3">
+        <v>-4.4477772024342716E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>1.2150806833280119E-3</v>
+      </c>
+      <c r="D4">
+        <v>6.3951960216055816E-3</v>
+      </c>
+      <c r="E4">
+        <v>-2.9162425232962192E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>2.5834804820276339E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.3939298887556699E-2</v>
+      </c>
+      <c r="E5">
+        <v>5.5481658634526244E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>-5.1288574949595964E-3</v>
+      </c>
+      <c r="D6">
+        <v>-6.7607949486560804E-3</v>
+      </c>
+      <c r="E6">
+        <v>6.616541040896783E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7">
+        <v>-3.5603341427601902E-2</v>
+      </c>
+      <c r="D7">
+        <v>-2.3688641347341579E-2</v>
+      </c>
+      <c r="E7">
+        <v>1.72860229105715E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8">
+        <v>3.9713388948112108E-3</v>
+      </c>
+      <c r="D8">
+        <v>-4.4284043368322239E-3</v>
+      </c>
+      <c r="E8">
+        <v>9.827795432620118E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>5.0969995340304907E-4</v>
+      </c>
+      <c r="D9">
+        <v>2.1988377787071048E-3</v>
+      </c>
+      <c r="E9">
+        <v>-3.2743078333541208E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>2.0395888926752039E-3</v>
+      </c>
+      <c r="D10">
+        <v>3.713510337770524E-3</v>
+      </c>
+      <c r="E10">
+        <v>-5.4443057841569006E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <v>-1.123327787851514E-3</v>
+      </c>
+      <c r="D11">
+        <v>-5.6198860657897588E-4</v>
+      </c>
+      <c r="E11">
+        <v>6.0739915665829837E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>-1.059950008335001E-2</v>
+      </c>
+      <c r="D12">
+        <v>3.8708908037089919E-4</v>
+      </c>
+      <c r="E12">
+        <v>1.393833423682379E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13">
+        <v>1.0076768496269669E-2</v>
+      </c>
+      <c r="D13">
+        <v>1.391505523484275E-2</v>
+      </c>
+      <c r="E13">
+        <v>-1.665933896132936E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14">
+        <v>7.3620041196364316E-5</v>
+      </c>
+      <c r="D14">
+        <v>1.168051005334184E-4</v>
+      </c>
+      <c r="E14">
+        <v>-2.6049739020856922E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15">
+        <v>-0.10050078190817539</v>
+      </c>
+      <c r="D15">
+        <v>-0.19011690259315531</v>
+      </c>
+      <c r="E15">
+        <v>4.0284787261861812E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16">
+        <v>4.2314416931838296E-3</v>
+      </c>
+      <c r="D16">
+        <v>1.2686338588434221E-3</v>
+      </c>
+      <c r="E16">
+        <v>-1.1119690939355451E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17">
+        <v>-3.528404991108082E-2</v>
+      </c>
+      <c r="D17">
+        <v>-1.1029499275027679E-2</v>
+      </c>
+      <c r="E17">
+        <v>2.7503766009568211E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18">
+        <v>5.7376527860799314E-3</v>
+      </c>
+      <c r="D18">
+        <v>1.202516181178228E-2</v>
+      </c>
+      <c r="E18">
+        <v>-2.5165433244864412E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>-2.2458813057737209E-3</v>
+      </c>
+      <c r="D19">
+        <v>-2.490784227500346E-3</v>
+      </c>
+      <c r="E19">
+        <v>2.4354565749736741E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20">
+        <v>-6.01245707143345E-4</v>
+      </c>
+      <c r="D20">
+        <v>-1.439567034477388E-4</v>
+      </c>
+      <c r="E20">
+        <v>-2.8993431613487722E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21">
+        <v>-4.537126098581837E-3</v>
+      </c>
+      <c r="D21">
+        <v>-8.9839247002082602E-3</v>
+      </c>
+      <c r="E21">
+        <v>1.4537007381350291E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>1.19480663645142E-4</v>
+      </c>
+      <c r="D22">
+        <v>2.5962204113096502E-3</v>
+      </c>
+      <c r="E22">
+        <v>-1.5850106484781041E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>4.508406913354494E-3</v>
+      </c>
+      <c r="E23">
+        <v>-1.452009463932221E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24">
+        <v>-7.1434800274582256E-3</v>
+      </c>
+      <c r="D24">
+        <v>-1.326488766069237E-2</v>
+      </c>
+      <c r="E24">
+        <v>2.511665500019908E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25">
+        <v>-7.6993249794996858E-3</v>
+      </c>
+      <c r="D25">
+        <v>-8.4308010795756984E-3</v>
+      </c>
+      <c r="E25">
+        <v>8.812070822980455E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27">
+        <v>-2.082922761381703E-3</v>
+      </c>
+      <c r="D27">
+        <v>-2.7961889467057939E-3</v>
+      </c>
+      <c r="E27">
+        <v>3.3472878692589799E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28">
+        <v>-3.0961769227570149E-3</v>
+      </c>
+      <c r="D28">
+        <v>-4.1873077332752924E-3</v>
+      </c>
+      <c r="E28">
+        <v>4.7534639441817349E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29">
+        <v>-1.031349575495564E-2</v>
+      </c>
+      <c r="D29">
+        <v>-7.2020100008796644E-3</v>
+      </c>
+      <c r="E29">
+        <v>5.7560700009284902E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30">
+        <v>5.0298295606789464E-3</v>
+      </c>
+      <c r="D30">
+        <v>5.1223657461429272E-3</v>
+      </c>
+      <c r="E30">
+        <v>-1.0233143546350019E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31">
+        <v>1.5910455213263699E-2</v>
+      </c>
+      <c r="D31">
+        <v>-2.8178221722153601E-2</v>
+      </c>
+      <c r="E31">
+        <v>2.7652847350962778E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32">
+        <v>-2.1622117667271731E-2</v>
+      </c>
+      <c r="D32">
+        <v>-2.385917261478843E-2</v>
+      </c>
+      <c r="E32">
+        <v>2.364193859014368E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33">
+        <v>-5.741359657127432E-3</v>
+      </c>
+      <c r="D33">
+        <v>-5.5767528176123883E-3</v>
+      </c>
+      <c r="E33">
+        <v>6.5345550353583493E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34">
+        <v>-1.1112888980814759E-3</v>
+      </c>
+      <c r="D34">
+        <v>-1.9737212873738399E-3</v>
+      </c>
+      <c r="E34">
+        <v>3.5030226150964492E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35">
+        <v>-2.4431632899919362E-3</v>
+      </c>
+      <c r="D35">
+        <v>-3.1040969241812829E-3</v>
+      </c>
+      <c r="E35">
+        <v>3.3898221910362911E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36">
+        <v>-5.490955221124574E-3</v>
+      </c>
+      <c r="D36">
+        <v>-9.3110712773736923E-3</v>
+      </c>
+      <c r="E36">
+        <v>1.397492294224634E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37">
+        <v>0.1179723419634733</v>
+      </c>
+      <c r="D37">
+        <v>0.13857867651592101</v>
+      </c>
+      <c r="E37">
+        <v>-6.2777422721609346E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>